<commit_message>
Script de validación de anulación de poliza por reemplazo. Correcciones en las validaciones de formularios
</commit_message>
<xml_diff>
--- a/Sura/DataSource - Cotización Motor.xlsx
+++ b/Sura/DataSource - Cotización Motor.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27757EB9-D8DB-4F56-B4AA-E772E68726FE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84322148-60EE-486C-A3BB-2AA06F59C5C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -108,9 +108,6 @@
     <t>FechaInicio</t>
   </si>
   <si>
-    <t>3 meses</t>
-  </si>
-  <si>
     <t>TipoTarjeta</t>
   </si>
   <si>
@@ -141,13 +138,16 @@
     <t>No</t>
   </si>
   <si>
-    <t>MMM111</t>
-  </si>
-  <si>
-    <t>MASDAS12312</t>
-  </si>
-  <si>
-    <t>ASDAKE1232</t>
+    <t>MMM115</t>
+  </si>
+  <si>
+    <t>MASDAS12316</t>
+  </si>
+  <si>
+    <t>ASDAKE1236</t>
+  </si>
+  <si>
+    <t>Anual</t>
   </si>
 </sst>
 </file>
@@ -499,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="W3" sqref="W3"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,7 +514,7 @@
     <col min="7" max="8" width="19.28515625" customWidth="1"/>
     <col min="9" max="9" width="14.85546875" customWidth="1"/>
     <col min="10" max="17" width="21.28515625" customWidth="1"/>
-    <col min="18" max="18" width="5.140625" customWidth="1"/>
+    <col min="18" max="18" width="6.7109375" customWidth="1"/>
     <col min="19" max="19" width="11.140625" customWidth="1"/>
     <col min="20" max="20" width="7.85546875" customWidth="1"/>
     <col min="21" max="21" width="11.5703125" customWidth="1"/>
@@ -560,19 +560,19 @@
         <v>22</v>
       </c>
       <c r="L1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" t="s">
         <v>28</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>29</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>30</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>31</v>
-      </c>
-      <c r="P1" t="s">
-        <v>32</v>
       </c>
       <c r="Q1" t="s">
         <v>26</v>
@@ -607,19 +607,19 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E2" s="3">
-        <v>9498924883</v>
+        <v>8684079401</v>
       </c>
       <c r="F2" t="s">
         <v>13</v>
@@ -628,13 +628,13 @@
         <v>16</v>
       </c>
       <c r="H2" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="I2" t="s">
         <v>17</v>
       </c>
       <c r="J2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K2" t="s">
         <v>23</v>
@@ -653,16 +653,16 @@
         <v>900000</v>
       </c>
       <c r="V2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="W2" t="s">
+        <v>37</v>
+      </c>
+      <c r="X2" t="s">
         <v>38</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>39</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>40</v>
       </c>
       <c r="Z2" t="s">
         <v>18</v>

</xml_diff>